<commit_message>
Update product evalution document
</commit_message>
<xml_diff>
--- a/document/schedule.xlsx
+++ b/document/schedule.xlsx
@@ -112,6 +112,7 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -174,7 +175,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -196,6 +197,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -287,13 +296,13 @@
   <dimension ref="A1:O65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="15" min="2" style="0" width="7.39271255060729"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="15" min="2" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -353,12 +362,12 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -366,8 +375,8 @@
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7" t="s">
+      <c r="E4" s="8"/>
+      <c r="F4" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -375,8 +384,8 @@
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7" t="s">
+      <c r="F5" s="8"/>
+      <c r="G5" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -384,8 +393,8 @@
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7" t="s">
+      <c r="G6" s="8"/>
+      <c r="H6" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -393,8 +402,8 @@
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7" t="s">
+      <c r="H7" s="8"/>
+      <c r="I7" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -402,8 +411,8 @@
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="7" t="s">
+      <c r="I8" s="8"/>
+      <c r="J8" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -411,8 +420,8 @@
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="7" t="s">
+      <c r="K9" s="8"/>
+      <c r="L9" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -420,8 +429,8 @@
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L10" s="6"/>
-      <c r="M10" s="7" t="s">
+      <c r="L10" s="8"/>
+      <c r="M10" s="9" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>